<commit_message>
Mejoras en el exportar excel
</commit_message>
<xml_diff>
--- a/exportado.xlsx
+++ b/exportado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,47 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>fecha inicio</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>hora</t>
+          <t>hora inicio</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>fecha final</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hora final</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Buenas</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Malas</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Porcentaje buenas</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo</t>
         </is>
       </c>
     </row>
@@ -461,19 +486,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>31-08-2023</t>
+          <t>21-10-2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>19:44:38</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
+          <t>01:36:13</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>21-10-2023</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01:36:13</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="n">
+        <v>30</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Foto</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -482,19 +528,124 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>31-08-2023</t>
+          <t>21-10-2023</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>22:38:24</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+          <t>01:48:39</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>21-10-2023</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>01:48:56</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
         <v>2</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>6</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" t="n">
+        <v>25</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>21-10-2023</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>01:52:26</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>21-10-2023</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>01:52:35</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>21-10-2023</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>02:11:22</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>21-10-2023</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>02:11:31</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Transmision</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>